<commit_message>
add vienna marmoset data; merge with pilot data
</commit_message>
<xml_diff>
--- a/data/raw_data/ManyPrimates_mp1_datasheet_Apenheul.xlsx
+++ b/data/raw_data/ManyPrimates_mp1_datasheet_Apenheul.xlsx
@@ -36,6 +36,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">formatted in the following way: YYYYMMDD (e.g. 20180131). </t>
     </r>
     <r>
@@ -98,6 +99,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">block number, </t>
     </r>
     <r>
@@ -107,6 +109,7 @@
       <t>continuous across sessions</t>
     </r>
     <r>
+      <rPr/>
       <t>. Each block must be three trials of the same delay type. Must be numeric</t>
     </r>
   </si>
@@ -115,6 +118,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">trial number, </t>
     </r>
     <r>
@@ -124,6 +128,7 @@
       <t>continuous across sessions</t>
     </r>
     <r>
+      <rPr/>
       <t xml:space="preserve"> (i.e., do not start again with 1). Must be numeric</t>
     </r>
   </si>
@@ -144,6 +149,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">first location indicated by subject </t>
     </r>
     <r>

</xml_diff>